<commit_message>
Adding Test data for Revlon UK
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
+++ b/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AB2E41-B537-4CAC-8079-920AB601ED61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A763C11F-63DD-4F41-A009-4F2B9CFEDCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t>UserName</t>
   </si>
@@ -70,9 +70,6 @@
     <t>phone</t>
   </si>
   <si>
-    <t>cardType</t>
-  </si>
-  <si>
     <t>cardNumber</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Guest_shipping</t>
   </si>
   <si>
-    <t>4444444444444448</t>
-  </si>
-  <si>
     <t>Dec</t>
   </si>
   <si>
@@ -259,7 +253,28 @@
     <t>1212121212121212</t>
   </si>
   <si>
-    <t>harish1@testmail.com</t>
+    <t>Retailer0112@gmail.com</t>
+  </si>
+  <si>
+    <t>Salon Performance Turbo</t>
+  </si>
+  <si>
+    <t>CardName</t>
+  </si>
+  <si>
+    <t>HARISH</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>03/30</t>
+  </si>
+  <si>
+    <t>Salon Straight Copper Smooth Styler</t>
+  </si>
+  <si>
+    <t>Retailer03121CC@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -320,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -330,6 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,7 +630,7 @@
   <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +647,7 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
@@ -667,10 +684,10 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>12</v>
@@ -685,52 +702,52 @@
         <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="S1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="W1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="Y1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="AB1" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -738,39 +755,39 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -779,22 +796,22 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
@@ -812,16 +829,16 @@
       </c>
       <c r="C5" s="1"/>
       <c r="N5" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="4">
-        <v>2021</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>53</v>
+        <v>81</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
       </c>
       <c r="R5" s="3">
         <v>737</v>
@@ -829,20 +846,20 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1"/>
       <c r="N6" t="s">
         <v>10</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P6" s="4">
         <v>2021</v>
       </c>
       <c r="Q6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R6" s="3">
         <v>737</v>
@@ -850,51 +867,51 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="S7" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="T7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
         <v>40</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" t="s">
-        <v>41</v>
       </c>
       <c r="L8">
         <v>12345</v>
@@ -903,16 +920,16 @@
         <v>9898989899</v>
       </c>
       <c r="S8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W8">
         <v>12341</v>
       </c>
       <c r="X8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y8" s="6">
         <v>5</v>
@@ -926,31 +943,31 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
         <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" t="s">
-        <v>41</v>
       </c>
       <c r="L9">
         <v>12345</v>
@@ -959,16 +976,16 @@
         <v>9898989899</v>
       </c>
       <c r="S9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W9">
         <v>12341</v>
       </c>
       <c r="X9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y9" s="6">
         <v>5</v>
@@ -982,114 +999,117 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" t="s">
         <v>61</v>
       </c>
-      <c r="H10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="L10" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="K10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
       </c>
+      <c r="S10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="S13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1124,7 @@
     <hyperlink ref="F10" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
     <hyperlink ref="F17" r:id="rId10" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{7326C0F6-32A8-49A4-8528-688B115248D7}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{28749BE0-4C33-4332-95CD-D48115062F68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>

</xml_diff>

<commit_message>
Revlon UK Expansion Test Cases for WEB & Mobile
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
+++ b/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A763C11F-63DD-4F41-A009-4F2B9CFEDCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F9E63C-48DE-471C-B04A-BD538CAEEE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
   <si>
     <t>UserName</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Guest_shipping</t>
-  </si>
-  <si>
-    <t>Dec</t>
   </si>
   <si>
     <t>Zero_Search</t>
@@ -335,12 +332,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -629,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,8 +651,8 @@
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="6"/>
+    <col min="25" max="25" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="9.140625" style="5"/>
     <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -702,7 +698,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>16</v>
@@ -734,20 +730,20 @@
       <c r="X1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -772,13 +768,13 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -787,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -829,13 +825,13 @@
       </c>
       <c r="C5" s="1"/>
       <c r="N5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="Q5">
         <v>12</v>
@@ -846,20 +842,20 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1"/>
       <c r="N6" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P6" s="4">
-        <v>2021</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>51</v>
+      <c r="O6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6">
+        <v>12</v>
       </c>
       <c r="R6" s="3">
         <v>737</v>
@@ -873,7 +869,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="S7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T7" t="s">
         <v>25</v>
@@ -931,13 +927,13 @@
       <c r="X8" t="s">
         <v>44</v>
       </c>
-      <c r="Y8" s="6">
+      <c r="Y8" s="5">
         <v>5</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="Z8" s="5">
         <v>6</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AA8" s="5">
         <v>2020</v>
       </c>
     </row>
@@ -987,13 +983,13 @@
       <c r="X9" t="s">
         <v>44</v>
       </c>
-      <c r="Y9" s="6">
+      <c r="Y9" s="5">
         <v>5</v>
       </c>
-      <c r="Z9" s="6">
+      <c r="Z9" s="5">
         <v>6</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AA9" s="5">
         <v>2020</v>
       </c>
     </row>
@@ -1011,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
         <v>39</v>
@@ -1020,38 +1016,38 @@
         <v>34</v>
       </c>
       <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" t="s">
         <v>60</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
       </c>
       <c r="S10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="S11" t="s">
         <v>52</v>
-      </c>
-      <c r="S11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1060,44 +1056,44 @@
         <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -1109,7 +1105,7 @@
         <v>28</v>
       </c>
       <c r="AC17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revlon UK Email triggering Code Latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
+++ b/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF541DB9-584E-4E68-885F-C905B50979CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D004E8-DACD-4EA6-9A6F-CB2100EA31BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>UserName</t>
   </si>
@@ -269,6 +269,42 @@
   </si>
   <si>
     <t>AB12 3CD</t>
+  </si>
+  <si>
+    <t>HeaderNames</t>
+  </si>
+  <si>
+    <t>HeaderLinks</t>
+  </si>
+  <si>
+    <t>One-Step,Straighteners,Dryers,Hair Stylers</t>
+  </si>
+  <si>
+    <t>ForgotPassword</t>
+  </si>
+  <si>
+    <t>Revlon Hair Tools &lt;Revlon@r1.dotdigital-email.com&gt;</t>
+  </si>
+  <si>
+    <t>Harish Chiruvella &lt;harish.chiruvella1@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Your Password Reset Request</t>
+  </si>
+  <si>
+    <t>Set a New Password</t>
+  </si>
+  <si>
+    <t>fromAddress</t>
+  </si>
+  <si>
+    <t>toAddress</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>content</t>
   </si>
 </sst>
 </file>
@@ -620,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,9 +688,14 @@
     <col min="26" max="27" width="9.140625" style="5"/>
     <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -742,8 +783,23 @@
       <c r="AC1" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -763,7 +819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -783,7 +839,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -816,7 +872,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -837,7 +893,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -858,7 +914,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -878,7 +934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -934,7 +990,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -990,7 +1046,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1028,7 +1084,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1036,7 +1092,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1056,7 +1112,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1064,7 +1120,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1072,7 +1128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1080,7 +1136,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1088,7 +1144,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1103,6 +1159,40 @@
       </c>
       <c r="AC17" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AE19" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1118,8 +1208,9 @@
     <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
     <hyperlink ref="F17" r:id="rId10" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
     <hyperlink ref="B3" r:id="rId11" xr:uid="{28749BE0-4C33-4332-95CD-D48115062F68}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revlon UK E-Comm and content latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
+++ b/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE85F1-439C-45AB-97F5-ADD22604C835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CA8424-6B36-4BC6-BC70-726471904958}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
   <si>
     <t>UserName</t>
   </si>
@@ -262,49 +262,49 @@
     <t>03/30</t>
   </si>
   <si>
+    <t>Retailer03121CC@gmail.com</t>
+  </si>
+  <si>
+    <t>AB12 3CD</t>
+  </si>
+  <si>
+    <t>HeaderNames</t>
+  </si>
+  <si>
+    <t>HeaderLinks</t>
+  </si>
+  <si>
+    <t>One-Step,Straighteners,Dryers,Hair Stylers</t>
+  </si>
+  <si>
+    <t>ForgotPassword</t>
+  </si>
+  <si>
+    <t>Revlon Hair Tools &lt;Revlon@r1.dotdigital-email.com&gt;</t>
+  </si>
+  <si>
+    <t>Harish Chiruvella &lt;harish.chiruvella1@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Your Password Reset Request</t>
+  </si>
+  <si>
+    <t>Set a New Password</t>
+  </si>
+  <si>
+    <t>fromAddress</t>
+  </si>
+  <si>
+    <t>toAddress</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
     <t>Salon Straight Copper Smooth Styler</t>
-  </si>
-  <si>
-    <t>Retailer03121CC@gmail.com</t>
-  </si>
-  <si>
-    <t>AB12 3CD</t>
-  </si>
-  <si>
-    <t>HeaderNames</t>
-  </si>
-  <si>
-    <t>HeaderLinks</t>
-  </si>
-  <si>
-    <t>One-Step,Straighteners,Dryers,Hair Stylers</t>
-  </si>
-  <si>
-    <t>ForgotPassword</t>
-  </si>
-  <si>
-    <t>Revlon Hair Tools &lt;Revlon@r1.dotdigital-email.com&gt;</t>
-  </si>
-  <si>
-    <t>Harish Chiruvella &lt;harish.chiruvella1@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>Your Password Reset Request</t>
-  </si>
-  <si>
-    <t>Set a New Password</t>
-  </si>
-  <si>
-    <t>fromAddress</t>
-  </si>
-  <si>
-    <t>toAddress</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>content</t>
   </si>
 </sst>
 </file>
@@ -656,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH20"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -784,19 +784,19 @@
         <v>70</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AE1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="S7" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
@@ -1075,7 +1075,7 @@
         <v>59</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
@@ -1163,15 +1163,15 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD18" t="s">
         <v>84</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1183,16 +1183,16 @@
       <c r="Z19"/>
       <c r="AA19"/>
       <c r="AE19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF19" t="s">
         <v>87</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AG19" t="s">
         <v>88</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
         <v>89</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -1212,23 +1212,44 @@
         <v>43</v>
       </c>
     </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
-    <hyperlink ref="U7" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
-    <hyperlink ref="V7" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{28749BE0-4C33-4332-95CD-D48115062F68}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
-    <hyperlink ref="F20" r:id="rId13" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="U7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="V7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F21" r:id="rId14" xr:uid="{5FAF22DE-F520-4C2A-A5B6-9B1A27D7E7EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RevlonUK New Expansion testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
+++ b/src/test/resources/TestData/revlonUK/RevlonUKTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CA8424-6B36-4BC6-BC70-726471904958}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D31768-6BDE-4AB3-8D43-8DC87403AEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
   <si>
     <t>UserName</t>
   </si>
@@ -262,6 +262,9 @@
     <t>03/30</t>
   </si>
   <si>
+    <t>Salon Straight Copper Smooth Styler</t>
+  </si>
+  <si>
     <t>Retailer03121CC@gmail.com</t>
   </si>
   <si>
@@ -304,7 +307,31 @@
     <t>content</t>
   </si>
   <si>
-    <t>Salon Straight Copper Smooth Styler</t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>chiruvella</t>
+  </si>
+  <si>
+    <t>855 Colony Dr crowley TX</t>
+  </si>
+  <si>
+    <t>florida</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>NewBillingAddress</t>
+  </si>
+  <si>
+    <t>harish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">655 N Gabriel Ave Newton NC </t>
+  </si>
+  <si>
+    <t>New Address</t>
   </si>
 </sst>
 </file>
@@ -656,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +706,7 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.42578125" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -695,7 +722,7 @@
     <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -784,22 +811,25 @@
         <v>70</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -819,7 +849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -836,10 +866,10 @@
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -872,7 +902,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -893,7 +923,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -914,7 +944,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -922,7 +952,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="S7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
@@ -933,8 +963,11 @@
       <c r="V7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -990,7 +1023,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1019,7 +1052,7 @@
         <v>39</v>
       </c>
       <c r="L9">
-        <v>12345</v>
+        <v>122345</v>
       </c>
       <c r="M9" s="3">
         <v>9898989899</v>
@@ -1046,7 +1079,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1075,7 +1108,7 @@
         <v>59</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
@@ -1084,7 +1117,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1092,7 +1125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1112,7 +1145,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1120,7 +1153,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1128,7 +1161,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1136,7 +1169,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1163,15 +1196,15 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AD18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1183,16 +1216,16 @@
       <c r="Z19"/>
       <c r="AA19"/>
       <c r="AE19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AF19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AG19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AH19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -1214,42 +1247,79 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
       </c>
       <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21">
+        <v>428658</v>
+      </c>
+      <c r="M21">
+        <v>5236987412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>71</v>
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22">
+        <v>799272</v>
+      </c>
+      <c r="M22">
+        <v>8523697415</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="U7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="V7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F21" r:id="rId14" xr:uid="{5FAF22DE-F520-4C2A-A5B6-9B1A27D7E7EF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
+    <hyperlink ref="U7" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
+    <hyperlink ref="V7" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{1E5A79C9-9C18-42C3-B520-7BD394A6C354}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{A338F397-E91C-4A0D-99EB-AF16E44EEA5A}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{28749BE0-4C33-4332-95CD-D48115062F68}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>